<commit_message>
added coauthor downloading, application downloading, added basic doc generation that doesn't work
</commit_message>
<xml_diff>
--- a/wp-content/plugins/wp-conference/stats/reports/reports.xlsx
+++ b/wp-content/plugins/wp-conference/stats/reports/reports.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Конференция</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Автор</t>
   </si>
   <si>
+    <t>Соавторы</t>
+  </si>
+  <si>
     <t>Название доклада</t>
   </si>
   <si>
@@ -36,6 +39,33 @@
   </si>
   <si>
     <t>Статус</t>
+  </si>
+  <si>
+    <t>РиМ-2021</t>
+  </si>
+  <si>
+    <t>Атомарные вычисления</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хмельный Никита </t>
+  </si>
+  <si>
+    <t>Штопор Александр. Евгеньевич, Торцев Петр. Константинович</t>
+  </si>
+  <si>
+    <t>ИИ в ИИ</t>
+  </si>
+  <si>
+    <t>На модерации</t>
+  </si>
+  <si>
+    <t>Хмельный_Никита_ИИ_в_ИИ_report.doc</t>
+  </si>
+  <si>
+    <t>Вождение пьяным за рулем</t>
+  </si>
+  <si>
+    <t>Хмельный_Никита_Вождение_пьяным_за_рулем_report.doc</t>
   </si>
 </sst>
 </file>
@@ -374,7 +404,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -382,7 +412,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,6 +433,57 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>